<commit_message>
updated evaluation and added graphs to each run for ncd
</commit_message>
<xml_diff>
--- a/json/archive/evaluation.xlsx
+++ b/json/archive/evaluation.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G91"/>
+  <dimension ref="A1:F91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -379,27 +379,22 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>average min_typicality</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>average_typicality with ncd (crit 1)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>criterion 2 with ncd</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>min_typicality</t>
-        </is>
-      </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
           <t>ncd_full</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>single_results average ncd</t>
         </is>
       </c>
     </row>
@@ -415,19 +410,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.6212962962962962</v>
+        <v>0.4581470588235295</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0.3787037037037038</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4581470588235295</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7037037037037037</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.6212962962962962</v>
+        <v>0.2962962962962963</v>
       </c>
     </row>
     <row r="3">
@@ -442,19 +434,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.6314814814814814</v>
+        <v>0.4265755565384047</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0.3685185185185186</v>
       </c>
       <c r="E3" t="n">
-        <v>0.4265755565384047</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6724137931034483</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.6314814814814815</v>
+        <v>0.3275862068965517</v>
       </c>
     </row>
     <row r="4">
@@ -469,19 +458,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.624074074074074</v>
+        <v>0.3962410990712074</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0.3759259259259259</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3962410990712074</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.7295081967213115</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.624074074074074</v>
+        <v>0.2704918032786885</v>
       </c>
     </row>
     <row r="5">
@@ -496,19 +482,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.6101851851851852</v>
+        <v>0.411</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>0.3898148148148148</v>
       </c>
       <c r="E5" t="n">
-        <v>0.411</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.7222222222222222</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.6101851851851852</v>
+        <v>0.2777777777777778</v>
       </c>
     </row>
     <row r="6">
@@ -523,19 +506,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.6212962962962962</v>
+        <v>0.4201544977640179</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0.3787037037037037</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4201544977640179</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7007874015748031</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.6212962962962962</v>
+        <v>0.2992125984251969</v>
       </c>
     </row>
     <row r="7">
@@ -550,19 +530,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.625925925925926</v>
+        <v>0.3959504213966288</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0.3740740740740741</v>
       </c>
       <c r="E7" t="n">
-        <v>0.3959504213966288</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.72</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.625925925925926</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="8">
@@ -577,19 +554,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.6138888888888889</v>
+        <v>0.3713888888888889</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>0.3861111111111111</v>
       </c>
       <c r="E8" t="n">
-        <v>0.3713888888888889</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.6851851851851852</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.6138888888888889</v>
+        <v>0.3148148148148148</v>
       </c>
     </row>
     <row r="9">
@@ -604,19 +578,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.6148148148148148</v>
+        <v>0.4018508771929825</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>0.3851851851851852</v>
       </c>
       <c r="E9" t="n">
-        <v>0.4018508771929825</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.7017543859649122</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.6148148148148149</v>
+        <v>0.2982456140350878</v>
       </c>
     </row>
     <row r="10">
@@ -631,19 +602,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.6166666666666666</v>
+        <v>0.4431787495700035</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>0.3833333333333334</v>
       </c>
       <c r="E10" t="n">
-        <v>0.4431787495700035</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.7037037037037037</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.6166666666666666</v>
+        <v>0.2962962962962963</v>
       </c>
     </row>
     <row r="11">
@@ -658,19 +626,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.6212962962962962</v>
+        <v>0.4581470588235295</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0.3787037037037038</v>
       </c>
       <c r="E11" t="n">
-        <v>0.4581470588235295</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.7037037037037037</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.6212962962962962</v>
+        <v>0.2962962962962963</v>
       </c>
     </row>
     <row r="12">
@@ -685,19 +650,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.6268518518518518</v>
+        <v>0.4243669590643274</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>0.3731481481481482</v>
       </c>
       <c r="E12" t="n">
-        <v>0.4243669590643274</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.6916666666666667</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.6268518518518518</v>
+        <v>0.3083333333333333</v>
       </c>
     </row>
     <row r="13">
@@ -712,19 +674,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.625</v>
+        <v>0.4066745786033711</v>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>0.375</v>
       </c>
       <c r="E13" t="n">
-        <v>0.4066745786033711</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.7339449541284404</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0.625</v>
+        <v>0.2660550458715596</v>
       </c>
     </row>
     <row r="14">
@@ -739,19 +698,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.6101851851851852</v>
+        <v>0.411</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>0.3898148148148148</v>
       </c>
       <c r="E14" t="n">
-        <v>0.411</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>0.7222222222222222</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0.6101851851851852</v>
+        <v>0.2777777777777778</v>
       </c>
     </row>
     <row r="15">
@@ -766,19 +722,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.6250000000000002</v>
+        <v>0.3923471423657182</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>0.3750000000000001</v>
       </c>
       <c r="E15" t="n">
-        <v>0.3923471423657182</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>0.6976744186046512</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0.625</v>
+        <v>0.3023255813953488</v>
       </c>
     </row>
     <row r="16">
@@ -793,19 +746,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.6194444444444445</v>
+        <v>0.4111659356725146</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>0.3805555555555556</v>
       </c>
       <c r="E16" t="n">
-        <v>0.4111659356725146</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.7016129032258065</v>
-      </c>
-      <c r="G16" t="n">
-        <v>0.6194444444444445</v>
+        <v>0.2983870967741935</v>
       </c>
     </row>
     <row r="17">
@@ -820,19 +770,16 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.6138888888888889</v>
+        <v>0.3713888888888889</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>0.3861111111111111</v>
       </c>
       <c r="E17" t="n">
-        <v>0.3713888888888889</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>0.6851851851851852</v>
-      </c>
-      <c r="G17" t="n">
-        <v>0.6138888888888889</v>
+        <v>0.3148148148148148</v>
       </c>
     </row>
     <row r="18">
@@ -847,19 +794,16 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.6185185185185185</v>
+        <v>0.4091427588579292</v>
       </c>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>0.3814814814814815</v>
       </c>
       <c r="E18" t="n">
-        <v>0.4091427588579292</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>0.7674418604651163</v>
-      </c>
-      <c r="G18" t="n">
-        <v>0.6185185185185185</v>
+        <v>0.2325581395348837</v>
       </c>
     </row>
     <row r="19">
@@ -874,19 +818,16 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.6157407407407408</v>
+        <v>0.4209573443412453</v>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>0.3842592592592592</v>
       </c>
       <c r="E19" t="n">
-        <v>0.4209573443412453</v>
+        <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>0.6859504132231405</v>
-      </c>
-      <c r="G19" t="n">
-        <v>0.6157407407407407</v>
+        <v>0.3140495867768595</v>
       </c>
     </row>
     <row r="20">
@@ -901,19 +842,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.1428571428571428</v>
+        <v>0.866</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>0.8571428571428574</v>
       </c>
       <c r="E20" t="n">
-        <v>0.866</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
-        <v>0.3770491803278688</v>
-      </c>
-      <c r="G20" t="n">
-        <v>0.1428571428571428</v>
+        <v>0.6229508196721312</v>
       </c>
     </row>
     <row r="21">
@@ -928,19 +866,16 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.2334474072647927</v>
+        <v>0.6151755279034691</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>0.7665525927352074</v>
       </c>
       <c r="E21" t="n">
-        <v>0.6151755279034691</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
-        <v>0.6578947368421053</v>
-      </c>
-      <c r="G21" t="n">
-        <v>0.2334474072647927</v>
+        <v>0.3421052631578947</v>
       </c>
     </row>
     <row r="22">
@@ -955,19 +890,16 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.2178248299319728</v>
+        <v>0.7022925407925408</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>0.7821751700680272</v>
       </c>
       <c r="E22" t="n">
-        <v>0.7022925407925408</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
-        <v>0.6583333333333333</v>
-      </c>
-      <c r="G22" t="n">
-        <v>0.2178248299319728</v>
+        <v>0.3416666666666667</v>
       </c>
     </row>
     <row r="23">
@@ -982,19 +914,16 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.1816326530612245</v>
+        <v>0.8644999999999999</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>0.8183673469387756</v>
       </c>
       <c r="E23" t="n">
-        <v>0.8644999999999999</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
-        <v>0.3770491803278688</v>
-      </c>
-      <c r="G23" t="n">
-        <v>0.1816326530612245</v>
+        <v>0.6229508196721312</v>
       </c>
     </row>
     <row r="24">
@@ -1009,19 +938,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.2336300520208083</v>
+        <v>0.6733552623846741</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>0.7663699479791918</v>
       </c>
       <c r="E24" t="n">
-        <v>0.6733552623846741</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
-        <v>0.6875</v>
-      </c>
-      <c r="G24" t="n">
-        <v>0.2336300520208083</v>
+        <v>0.3125</v>
       </c>
     </row>
     <row r="25">
@@ -1036,19 +962,16 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.2335862344937976</v>
+        <v>0.6813813319033908</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>0.7664137655062025</v>
       </c>
       <c r="E25" t="n">
-        <v>0.6813813319033908</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
-        <v>0.6640625</v>
-      </c>
-      <c r="G25" t="n">
-        <v>0.2335862344937976</v>
+        <v>0.3359375</v>
       </c>
     </row>
     <row r="26">
@@ -1063,19 +986,16 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.1783265306122448</v>
+        <v>0.9435</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>0.8216734693877553</v>
       </c>
       <c r="E26" t="n">
-        <v>0.9435</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
-        <v>0.3387096774193548</v>
-      </c>
-      <c r="G26" t="n">
-        <v>0.1783265306122449</v>
+        <v>0.6612903225806452</v>
       </c>
     </row>
     <row r="27">
@@ -1090,19 +1010,16 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.2109975990396158</v>
+        <v>0.7469478854478855</v>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>0.7890024009603842</v>
       </c>
       <c r="E27" t="n">
-        <v>0.7469478854478855</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
-        <v>0.6428571428571429</v>
-      </c>
-      <c r="G27" t="n">
-        <v>0.2109975990396158</v>
+        <v>0.3571428571428571</v>
       </c>
     </row>
     <row r="28">
@@ -1117,19 +1034,16 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.2158074229691877</v>
+        <v>0.745111888111888</v>
       </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>0.7841925770308122</v>
       </c>
       <c r="E28" t="n">
-        <v>0.745111888111888</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-      <c r="G28" t="n">
-        <v>0.2158074229691877</v>
+        <v>0.3333333333333334</v>
       </c>
     </row>
     <row r="29">
@@ -1144,19 +1058,16 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.1428571428571428</v>
+        <v>0.866</v>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>0.8571428571428574</v>
       </c>
       <c r="E29" t="n">
-        <v>0.866</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
-        <v>0.3770491803278688</v>
-      </c>
-      <c r="G29" t="n">
-        <v>0.1428571428571428</v>
+        <v>0.6229508196721312</v>
       </c>
     </row>
     <row r="30">
@@ -1171,19 +1082,16 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.213561824729892</v>
+        <v>0.7183583916083917</v>
       </c>
       <c r="D30" t="n">
-        <v>0</v>
+        <v>0.786438175270108</v>
       </c>
       <c r="E30" t="n">
-        <v>0.7183583916083917</v>
+        <v>1</v>
       </c>
       <c r="F30" t="n">
-        <v>0.6639344262295082</v>
-      </c>
-      <c r="G30" t="n">
-        <v>0.213561824729892</v>
+        <v>0.3360655737704918</v>
       </c>
     </row>
     <row r="31">
@@ -1198,19 +1106,16 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.2190816326530612</v>
+        <v>0.7082170745920746</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>0.7809183673469386</v>
       </c>
       <c r="E31" t="n">
-        <v>0.7082170745920746</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-      <c r="G31" t="n">
-        <v>0.2190816326530612</v>
+        <v>0.3333333333333334</v>
       </c>
     </row>
     <row r="32">
@@ -1225,19 +1130,16 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.1816326530612245</v>
+        <v>0.8644999999999999</v>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>0.8183673469387756</v>
       </c>
       <c r="E32" t="n">
-        <v>0.8644999999999999</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
-        <v>0.3770491803278688</v>
-      </c>
-      <c r="G32" t="n">
-        <v>0.1816326530612245</v>
+        <v>0.6229508196721312</v>
       </c>
     </row>
     <row r="33">
@@ -1252,19 +1154,16 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.2157833133253301</v>
+        <v>0.77968006993007</v>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>0.7842166866746698</v>
       </c>
       <c r="E33" t="n">
-        <v>0.77968006993007</v>
+        <v>1</v>
       </c>
       <c r="F33" t="n">
-        <v>0.631578947368421</v>
-      </c>
-      <c r="G33" t="n">
-        <v>0.2157833133253301</v>
+        <v>0.368421052631579</v>
       </c>
     </row>
     <row r="34">
@@ -1279,19 +1178,16 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.2168065226090436</v>
+        <v>0.7372409257409258</v>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>0.7831934773909563</v>
       </c>
       <c r="E34" t="n">
-        <v>0.7372409257409258</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
-        <v>0.6694915254237288</v>
-      </c>
-      <c r="G34" t="n">
-        <v>0.2168065226090436</v>
+        <v>0.3305084745762712</v>
       </c>
     </row>
     <row r="35">
@@ -1306,19 +1202,16 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.1783265306122448</v>
+        <v>0.9435</v>
       </c>
       <c r="D35" t="n">
-        <v>0</v>
+        <v>0.8216734693877553</v>
       </c>
       <c r="E35" t="n">
-        <v>0.9435</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
-        <v>0.3387096774193548</v>
-      </c>
-      <c r="G35" t="n">
-        <v>0.1783265306122449</v>
+        <v>0.6612903225806452</v>
       </c>
     </row>
     <row r="36">
@@ -1333,19 +1226,16 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.222030412164866</v>
+        <v>0.6918720837985545</v>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>0.777969587835134</v>
       </c>
       <c r="E36" t="n">
-        <v>0.6918720837985545</v>
+        <v>1</v>
       </c>
       <c r="F36" t="n">
-        <v>0.6410256410256411</v>
-      </c>
-      <c r="G36" t="n">
-        <v>0.222030412164866</v>
+        <v>0.3589743589743589</v>
       </c>
     </row>
     <row r="37">
@@ -1360,19 +1250,16 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.2095729291716686</v>
+        <v>0.7382124125874124</v>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>0.7904270708283313</v>
       </c>
       <c r="E37" t="n">
-        <v>0.7382124125874124</v>
+        <v>1</v>
       </c>
       <c r="F37" t="n">
-        <v>0.6585365853658537</v>
-      </c>
-      <c r="G37" t="n">
-        <v>0.2095729291716687</v>
+        <v>0.3414634146341463</v>
       </c>
     </row>
     <row r="38">
@@ -1387,19 +1274,16 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.391304347826087</v>
+        <v>0.5941666666666667</v>
       </c>
       <c r="D38" t="n">
-        <v>0</v>
+        <v>0.6086956521739131</v>
       </c>
       <c r="E38" t="n">
-        <v>0.5941666666666667</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
-        <v>0.463768115942029</v>
-      </c>
-      <c r="G38" t="n">
-        <v>0.391304347826087</v>
+        <v>0.536231884057971</v>
       </c>
     </row>
     <row r="39">
@@ -1414,19 +1298,16 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.4318840579710145</v>
+        <v>0.5678351648351648</v>
       </c>
       <c r="D39" t="n">
-        <v>0</v>
+        <v>0.5681159420289854</v>
       </c>
       <c r="E39" t="n">
-        <v>0.5678351648351648</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
-        <v>0.6637931034482759</v>
-      </c>
-      <c r="G39" t="n">
-        <v>0.4318840579710145</v>
+        <v>0.3362068965517241</v>
       </c>
     </row>
     <row r="40">
@@ -1441,19 +1322,16 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.4260869565217391</v>
+        <v>0.5556693420958126</v>
       </c>
       <c r="D40" t="n">
-        <v>0</v>
+        <v>0.5739130434782609</v>
       </c>
       <c r="E40" t="n">
-        <v>0.5556693420958126</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
-        <v>0.6495726495726496</v>
-      </c>
-      <c r="G40" t="n">
-        <v>0.4260869565217392</v>
+        <v>0.3504273504273504</v>
       </c>
     </row>
     <row r="41">
@@ -1468,19 +1346,16 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.3797101449275362</v>
+        <v>0.5524230769230769</v>
       </c>
       <c r="D41" t="n">
-        <v>0</v>
+        <v>0.6202898550724638</v>
       </c>
       <c r="E41" t="n">
-        <v>0.5524230769230769</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
-        <v>0.4492753623188406</v>
-      </c>
-      <c r="G41" t="n">
-        <v>0.3797101449275362</v>
+        <v>0.5507246376811594</v>
       </c>
     </row>
     <row r="42">
@@ -1495,19 +1370,16 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.4202898550724637</v>
+        <v>0.5202584033613447</v>
       </c>
       <c r="D42" t="n">
-        <v>0</v>
+        <v>0.5797101449275361</v>
       </c>
       <c r="E42" t="n">
-        <v>0.5202584033613447</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
-        <v>0.6904761904761905</v>
-      </c>
-      <c r="G42" t="n">
-        <v>0.4202898550724637</v>
+        <v>0.3095238095238095</v>
       </c>
     </row>
     <row r="43">
@@ -1522,19 +1394,16 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0.4217391304347826</v>
+        <v>0.5661785714285714</v>
       </c>
       <c r="D43" t="n">
-        <v>0</v>
+        <v>0.5782608695652174</v>
       </c>
       <c r="E43" t="n">
-        <v>0.5661785714285714</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
-        <v>0.6854838709677419</v>
-      </c>
-      <c r="G43" t="n">
-        <v>0.4217391304347826</v>
+        <v>0.3145161290322581</v>
       </c>
     </row>
     <row r="44">
@@ -1549,19 +1418,16 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.4043478260869565</v>
+        <v>0.538</v>
       </c>
       <c r="D44" t="n">
-        <v>0</v>
+        <v>0.5956521739130435</v>
       </c>
       <c r="E44" t="n">
-        <v>0.538</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
-        <v>0.4492753623188406</v>
-      </c>
-      <c r="G44" t="n">
-        <v>0.4043478260869565</v>
+        <v>0.5507246376811594</v>
       </c>
     </row>
     <row r="45">
@@ -1576,19 +1442,16 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0.4144927536231885</v>
+        <v>0.5443131868131867</v>
       </c>
       <c r="D45" t="n">
-        <v>0</v>
+        <v>0.5855072463768115</v>
       </c>
       <c r="E45" t="n">
-        <v>0.5443131868131867</v>
+        <v>1</v>
       </c>
       <c r="F45" t="n">
-        <v>0.6833333333333333</v>
-      </c>
-      <c r="G45" t="n">
-        <v>0.4144927536231885</v>
+        <v>0.3166666666666667</v>
       </c>
     </row>
     <row r="46">
@@ -1603,19 +1466,16 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.4202898550724637</v>
+        <v>0.4823055555555557</v>
       </c>
       <c r="D46" t="n">
-        <v>0</v>
+        <v>0.5797101449275361</v>
       </c>
       <c r="E46" t="n">
-        <v>0.4823055555555557</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
-        <v>0.6837606837606838</v>
-      </c>
-      <c r="G46" t="n">
-        <v>0.4202898550724637</v>
+        <v>0.3162393162393162</v>
       </c>
     </row>
     <row r="47">
@@ -1630,19 +1490,16 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.391304347826087</v>
+        <v>0.5941666666666667</v>
       </c>
       <c r="D47" t="n">
-        <v>0</v>
+        <v>0.6086956521739131</v>
       </c>
       <c r="E47" t="n">
-        <v>0.5941666666666667</v>
+        <v>1</v>
       </c>
       <c r="F47" t="n">
-        <v>0.463768115942029</v>
-      </c>
-      <c r="G47" t="n">
-        <v>0.391304347826087</v>
+        <v>0.536231884057971</v>
       </c>
     </row>
     <row r="48">
@@ -1657,19 +1514,16 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>0.4362318840579711</v>
+        <v>0.5517011197866462</v>
       </c>
       <c r="D48" t="n">
-        <v>0.1</v>
+        <v>0.5637681159420289</v>
       </c>
       <c r="E48" t="n">
-        <v>0.5517011197866462</v>
+        <v>0.9</v>
       </c>
       <c r="F48" t="n">
-        <v>0.6692913385826772</v>
-      </c>
-      <c r="G48" t="n">
-        <v>0.436231884057971</v>
+        <v>0.3307086614173228</v>
       </c>
     </row>
     <row r="49">
@@ -1684,19 +1538,16 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.4057971014492754</v>
+        <v>0.5718655462184874</v>
       </c>
       <c r="D49" t="n">
-        <v>0</v>
+        <v>0.5942028985507246</v>
       </c>
       <c r="E49" t="n">
-        <v>0.5718655462184874</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
-        <v>0.6774193548387096</v>
-      </c>
-      <c r="G49" t="n">
-        <v>0.4057971014492754</v>
+        <v>0.3225806451612904</v>
       </c>
     </row>
     <row r="50">
@@ -1711,19 +1562,16 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.3797101449275362</v>
+        <v>0.5524230769230769</v>
       </c>
       <c r="D50" t="n">
-        <v>0</v>
+        <v>0.6202898550724638</v>
       </c>
       <c r="E50" t="n">
-        <v>0.5524230769230769</v>
+        <v>1</v>
       </c>
       <c r="F50" t="n">
-        <v>0.4492753623188406</v>
-      </c>
-      <c r="G50" t="n">
-        <v>0.3797101449275362</v>
+        <v>0.5507246376811594</v>
       </c>
     </row>
     <row r="51">
@@ -1738,19 +1586,16 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.4115942028985507</v>
+        <v>0.5462588522588522</v>
       </c>
       <c r="D51" t="n">
-        <v>0</v>
+        <v>0.5884057971014492</v>
       </c>
       <c r="E51" t="n">
-        <v>0.5462588522588522</v>
+        <v>1</v>
       </c>
       <c r="F51" t="n">
-        <v>0.6528925619834711</v>
-      </c>
-      <c r="G51" t="n">
-        <v>0.4115942028985508</v>
+        <v>0.3471074380165289</v>
       </c>
     </row>
     <row r="52">
@@ -1765,19 +1610,16 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0.4</v>
+        <v>0.589478021978022</v>
       </c>
       <c r="D52" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="E52" t="n">
-        <v>0.589478021978022</v>
+        <v>1</v>
       </c>
       <c r="F52" t="n">
-        <v>0.6403508771929824</v>
-      </c>
-      <c r="G52" t="n">
-        <v>0.4</v>
+        <v>0.3596491228070176</v>
       </c>
     </row>
     <row r="53">
@@ -1792,19 +1634,16 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0.4043478260869565</v>
+        <v>0.538</v>
       </c>
       <c r="D53" t="n">
-        <v>0</v>
+        <v>0.5956521739130435</v>
       </c>
       <c r="E53" t="n">
-        <v>0.538</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
-        <v>0.4492753623188406</v>
-      </c>
-      <c r="G53" t="n">
-        <v>0.4043478260869565</v>
+        <v>0.5507246376811594</v>
       </c>
     </row>
     <row r="54">
@@ -1819,19 +1658,16 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>0.4202898550724637</v>
+        <v>0.5303541083099907</v>
       </c>
       <c r="D54" t="n">
-        <v>0</v>
+        <v>0.5797101449275361</v>
       </c>
       <c r="E54" t="n">
-        <v>0.5303541083099907</v>
+        <v>1</v>
       </c>
       <c r="F54" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-      <c r="G54" t="n">
-        <v>0.4202898550724637</v>
+        <v>0.3333333333333334</v>
       </c>
     </row>
     <row r="55">
@@ -1846,19 +1682,16 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>0.4318840579710145</v>
+        <v>0.5065027826920242</v>
       </c>
       <c r="D55" t="n">
-        <v>0</v>
+        <v>0.5681159420289854</v>
       </c>
       <c r="E55" t="n">
-        <v>0.5065027826920242</v>
+        <v>1</v>
       </c>
       <c r="F55" t="n">
-        <v>0.7007874015748031</v>
-      </c>
-      <c r="G55" t="n">
-        <v>0.4318840579710145</v>
+        <v>0.2992125984251969</v>
       </c>
     </row>
     <row r="56">
@@ -1873,19 +1706,16 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0.5119047619047619</v>
+        <v>0.5199999999999999</v>
       </c>
       <c r="D56" t="n">
-        <v>1</v>
+        <v>0.4880952380952381</v>
       </c>
       <c r="E56" t="n">
-        <v>0.5199999999999999</v>
+        <v>0</v>
       </c>
       <c r="F56" t="n">
-        <v>0.5952380952380952</v>
-      </c>
-      <c r="G56" t="n">
-        <v>0.5119047619047619</v>
+        <v>0.4047619047619048</v>
       </c>
     </row>
     <row r="57">
@@ -1900,19 +1730,16 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>0.5142857142857143</v>
+        <v>0.4814332645338838</v>
       </c>
       <c r="D57" t="n">
-        <v>0.6</v>
+        <v>0.4857142857142857</v>
       </c>
       <c r="E57" t="n">
-        <v>0.4814332645338838</v>
+        <v>0.2</v>
       </c>
       <c r="F57" t="n">
-        <v>0.6166666666666667</v>
-      </c>
-      <c r="G57" t="n">
-        <v>0.5142857142857143</v>
+        <v>0.3833333333333333</v>
       </c>
     </row>
     <row r="58">
@@ -1927,19 +1754,16 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>0.5178571428571428</v>
+        <v>0.4686951754385965</v>
       </c>
       <c r="D58" t="n">
-        <v>0.8</v>
+        <v>0.4821428571428572</v>
       </c>
       <c r="E58" t="n">
-        <v>0.4686951754385965</v>
+        <v>0.1</v>
       </c>
       <c r="F58" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="G58" t="n">
-        <v>0.5178571428571428</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="59">
@@ -1954,19 +1778,16 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>0.5023809523809524</v>
+        <v>0.4826691176470589</v>
       </c>
       <c r="D59" t="n">
-        <v>0.1</v>
+        <v>0.4976190476190476</v>
       </c>
       <c r="E59" t="n">
-        <v>0.4826691176470589</v>
+        <v>0</v>
       </c>
       <c r="F59" t="n">
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="G59" t="n">
-        <v>0.5023809523809524</v>
+        <v>0.4285714285714286</v>
       </c>
     </row>
     <row r="60">
@@ -1981,19 +1802,16 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>0.5095238095238095</v>
+        <v>0.4634060457516339</v>
       </c>
       <c r="D60" t="n">
-        <v>0.5</v>
+        <v>0.4904761904761905</v>
       </c>
       <c r="E60" t="n">
-        <v>0.4634060457516339</v>
+        <v>0.3</v>
       </c>
       <c r="F60" t="n">
-        <v>0.6774193548387096</v>
-      </c>
-      <c r="G60" t="n">
-        <v>0.5095238095238095</v>
+        <v>0.3225806451612904</v>
       </c>
     </row>
     <row r="61">
@@ -2008,19 +1826,16 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>0.5166666666666666</v>
+        <v>0.4771241830065359</v>
       </c>
       <c r="D61" t="n">
-        <v>0.8</v>
+        <v>0.4833333333333333</v>
       </c>
       <c r="E61" t="n">
-        <v>0.4771241830065359</v>
+        <v>0</v>
       </c>
       <c r="F61" t="n">
-        <v>0.6517857142857143</v>
-      </c>
-      <c r="G61" t="n">
-        <v>0.5166666666666666</v>
+        <v>0.3482142857142857</v>
       </c>
     </row>
     <row r="62">
@@ -2035,19 +1850,16 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>0.4904761904761904</v>
+        <v>0.4597105263157896</v>
       </c>
       <c r="D62" t="n">
-        <v>0.1</v>
+        <v>0.5095238095238095</v>
       </c>
       <c r="E62" t="n">
-        <v>0.4597105263157896</v>
+        <v>0.9</v>
       </c>
       <c r="F62" t="n">
-        <v>0.5833333333333334</v>
-      </c>
-      <c r="G62" t="n">
-        <v>0.4904761904761904</v>
+        <v>0.4166666666666666</v>
       </c>
     </row>
     <row r="63">
@@ -2062,19 +1874,16 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>0.5202380952380953</v>
+        <v>0.4894685143288084</v>
       </c>
       <c r="D63" t="n">
-        <v>0.9</v>
+        <v>0.4797619047619047</v>
       </c>
       <c r="E63" t="n">
-        <v>0.4894685143288084</v>
+        <v>0.1</v>
       </c>
       <c r="F63" t="n">
-        <v>0.6470588235294118</v>
-      </c>
-      <c r="G63" t="n">
-        <v>0.5202380952380952</v>
+        <v>0.3529411764705882</v>
       </c>
     </row>
     <row r="64">
@@ -2089,19 +1898,16 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>0.519047619047619</v>
+        <v>0.4914876590987273</v>
       </c>
       <c r="D64" t="n">
-        <v>0.8</v>
+        <v>0.4809523809523809</v>
       </c>
       <c r="E64" t="n">
-        <v>0.4914876590987273</v>
+        <v>0</v>
       </c>
       <c r="F64" t="n">
-        <v>0.6916666666666667</v>
-      </c>
-      <c r="G64" t="n">
-        <v>0.519047619047619</v>
+        <v>0.3083333333333333</v>
       </c>
     </row>
     <row r="65">
@@ -2116,19 +1922,16 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>0.5119047619047619</v>
+        <v>0.5199999999999999</v>
       </c>
       <c r="D65" t="n">
-        <v>1</v>
+        <v>0.4880952380952381</v>
       </c>
       <c r="E65" t="n">
-        <v>0.5199999999999999</v>
+        <v>0</v>
       </c>
       <c r="F65" t="n">
-        <v>0.5952380952380952</v>
-      </c>
-      <c r="G65" t="n">
-        <v>0.5119047619047619</v>
+        <v>0.4047619047619048</v>
       </c>
     </row>
     <row r="66">
@@ -2143,19 +1946,16 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>0.5214285714285714</v>
+        <v>0.417922385620915</v>
       </c>
       <c r="D66" t="n">
-        <v>0.8</v>
+        <v>0.4785714285714286</v>
       </c>
       <c r="E66" t="n">
-        <v>0.417922385620915</v>
+        <v>0.1</v>
       </c>
       <c r="F66" t="n">
-        <v>0.6744186046511628</v>
-      </c>
-      <c r="G66" t="n">
-        <v>0.5214285714285714</v>
+        <v>0.3255813953488372</v>
       </c>
     </row>
     <row r="67">
@@ -2170,19 +1970,16 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>0.5190476190476191</v>
+        <v>0.4656897574819402</v>
       </c>
       <c r="D67" t="n">
-        <v>0.6</v>
+        <v>0.4809523809523809</v>
       </c>
       <c r="E67" t="n">
-        <v>0.4656897574819402</v>
+        <v>0.2</v>
       </c>
       <c r="F67" t="n">
-        <v>0.6341463414634146</v>
-      </c>
-      <c r="G67" t="n">
-        <v>0.519047619047619</v>
+        <v>0.3658536585365854</v>
       </c>
     </row>
     <row r="68">
@@ -2197,19 +1994,16 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>0.5023809523809524</v>
+        <v>0.4826691176470589</v>
       </c>
       <c r="D68" t="n">
-        <v>0.1</v>
+        <v>0.4976190476190476</v>
       </c>
       <c r="E68" t="n">
-        <v>0.4826691176470589</v>
+        <v>0</v>
       </c>
       <c r="F68" t="n">
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="G68" t="n">
-        <v>0.5023809523809524</v>
+        <v>0.4285714285714286</v>
       </c>
     </row>
     <row r="69">
@@ -2224,19 +2018,16 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>0.5261904761904762</v>
+        <v>0.4329419381787803</v>
       </c>
       <c r="D69" t="n">
-        <v>0.8</v>
+        <v>0.4738095238095238</v>
       </c>
       <c r="E69" t="n">
-        <v>0.4329419381787803</v>
+        <v>0.1</v>
       </c>
       <c r="F69" t="n">
-        <v>0.6554621848739496</v>
-      </c>
-      <c r="G69" t="n">
-        <v>0.5261904761904761</v>
+        <v>0.3445378151260504</v>
       </c>
     </row>
     <row r="70">
@@ -2251,19 +2042,16 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>0.5178571428571428</v>
+        <v>0.4644850852621751</v>
       </c>
       <c r="D70" t="n">
-        <v>0.7</v>
+        <v>0.4821428571428572</v>
       </c>
       <c r="E70" t="n">
-        <v>0.4644850852621751</v>
+        <v>0.2</v>
       </c>
       <c r="F70" t="n">
-        <v>0.7045454545454546</v>
-      </c>
-      <c r="G70" t="n">
-        <v>0.5178571428571429</v>
+        <v>0.2954545454545454</v>
       </c>
     </row>
     <row r="71">
@@ -2278,19 +2066,16 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>0.4904761904761904</v>
+        <v>0.4597105263157896</v>
       </c>
       <c r="D71" t="n">
-        <v>0.1</v>
+        <v>0.5095238095238095</v>
       </c>
       <c r="E71" t="n">
-        <v>0.4597105263157896</v>
+        <v>0.9</v>
       </c>
       <c r="F71" t="n">
-        <v>0.5833333333333334</v>
-      </c>
-      <c r="G71" t="n">
-        <v>0.4904761904761904</v>
+        <v>0.4166666666666666</v>
       </c>
     </row>
     <row r="72">
@@ -2305,19 +2090,16 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>0.5249999999999999</v>
+        <v>0.4840852253181975</v>
       </c>
       <c r="D72" t="n">
-        <v>0.9</v>
+        <v>0.4750000000000001</v>
       </c>
       <c r="E72" t="n">
-        <v>0.4840852253181975</v>
+        <v>0</v>
       </c>
       <c r="F72" t="n">
-        <v>0.7086614173228346</v>
-      </c>
-      <c r="G72" t="n">
-        <v>0.525</v>
+        <v>0.2913385826771654</v>
       </c>
     </row>
     <row r="73">
@@ -2332,19 +2114,16 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>0.5202380952380952</v>
+        <v>0.4572646198830409</v>
       </c>
       <c r="D73" t="n">
-        <v>0.7</v>
+        <v>0.4797619047619048</v>
       </c>
       <c r="E73" t="n">
-        <v>0.4572646198830409</v>
+        <v>0.1</v>
       </c>
       <c r="F73" t="n">
-        <v>0.7230769230769231</v>
-      </c>
-      <c r="G73" t="n">
-        <v>0.5202380952380952</v>
+        <v>0.2769230769230769</v>
       </c>
     </row>
     <row r="74">
@@ -2359,19 +2138,16 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>0.584375</v>
+        <v>0.4245789473684209</v>
       </c>
       <c r="D74" t="n">
-        <v>1</v>
+        <v>0.4156249999999999</v>
       </c>
       <c r="E74" t="n">
-        <v>0.4245789473684209</v>
+        <v>0</v>
       </c>
       <c r="F74" t="n">
-        <v>0.6354166666666666</v>
-      </c>
-      <c r="G74" t="n">
-        <v>0.584375</v>
+        <v>0.3645833333333334</v>
       </c>
     </row>
     <row r="75">
@@ -2386,19 +2162,16 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>0.590625</v>
+        <v>0.4649940925087983</v>
       </c>
       <c r="D75" t="n">
-        <v>1</v>
+        <v>0.4093749999999999</v>
       </c>
       <c r="E75" t="n">
-        <v>0.4649940925087983</v>
+        <v>0</v>
       </c>
       <c r="F75" t="n">
-        <v>0.6615384615384615</v>
-      </c>
-      <c r="G75" t="n">
-        <v>0.5906250000000001</v>
+        <v>0.3384615384615385</v>
       </c>
     </row>
     <row r="76">
@@ -2413,19 +2186,16 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>0.584375</v>
+        <v>0.4556924848886922</v>
       </c>
       <c r="D76" t="n">
-        <v>1</v>
+        <v>0.415625</v>
       </c>
       <c r="E76" t="n">
-        <v>0.4556924848886922</v>
+        <v>0</v>
       </c>
       <c r="F76" t="n">
-        <v>0.7079646017699115</v>
-      </c>
-      <c r="G76" t="n">
-        <v>0.584375</v>
+        <v>0.2920353982300885</v>
       </c>
     </row>
     <row r="77">
@@ -2440,19 +2210,16 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>0.5645833333333333</v>
+        <v>0.4321666666666666</v>
       </c>
       <c r="D77" t="n">
-        <v>1</v>
+        <v>0.4354166666666667</v>
       </c>
       <c r="E77" t="n">
-        <v>0.4321666666666666</v>
+        <v>0</v>
       </c>
       <c r="F77" t="n">
-        <v>0.6354166666666666</v>
-      </c>
-      <c r="G77" t="n">
-        <v>0.5645833333333333</v>
+        <v>0.3645833333333334</v>
       </c>
     </row>
     <row r="78">
@@ -2467,19 +2234,16 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>0.5822916666666667</v>
+        <v>0.4230421826625387</v>
       </c>
       <c r="D78" t="n">
-        <v>1</v>
+        <v>0.4177083333333334</v>
       </c>
       <c r="E78" t="n">
-        <v>0.4230421826625387</v>
+        <v>0</v>
       </c>
       <c r="F78" t="n">
-        <v>0.7153846153846154</v>
-      </c>
-      <c r="G78" t="n">
-        <v>0.5822916666666667</v>
+        <v>0.2846153846153846</v>
       </c>
     </row>
     <row r="79">
@@ -2494,19 +2258,16 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>0.584375</v>
+        <v>0.4563880718954249</v>
       </c>
       <c r="D79" t="n">
-        <v>1</v>
+        <v>0.415625</v>
       </c>
       <c r="E79" t="n">
-        <v>0.4563880718954249</v>
+        <v>0</v>
       </c>
       <c r="F79" t="n">
-        <v>0.6796875</v>
-      </c>
-      <c r="G79" t="n">
-        <v>0.584375</v>
+        <v>0.3203125</v>
       </c>
     </row>
     <row r="80">
@@ -2521,19 +2282,16 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>0.5927083333333333</v>
+        <v>0.5069705882352943</v>
       </c>
       <c r="D80" t="n">
-        <v>1</v>
+        <v>0.4072916666666667</v>
       </c>
       <c r="E80" t="n">
-        <v>0.5069705882352943</v>
+        <v>0</v>
       </c>
       <c r="F80" t="n">
-        <v>0.6458333333333334</v>
-      </c>
-      <c r="G80" t="n">
-        <v>0.5927083333333333</v>
+        <v>0.3541666666666666</v>
       </c>
     </row>
     <row r="81">
@@ -2548,19 +2306,16 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>0.5875</v>
+        <v>0.4393027605779154</v>
       </c>
       <c r="D81" t="n">
-        <v>1</v>
+        <v>0.4125</v>
       </c>
       <c r="E81" t="n">
-        <v>0.4393027605779154</v>
+        <v>0</v>
       </c>
       <c r="F81" t="n">
-        <v>0.7016129032258065</v>
-      </c>
-      <c r="G81" t="n">
-        <v>0.5875</v>
+        <v>0.2983870967741935</v>
       </c>
     </row>
     <row r="82">
@@ -2575,19 +2330,16 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>0.5927083333333333</v>
+        <v>0.4327913226694187</v>
       </c>
       <c r="D82" t="n">
-        <v>1</v>
+        <v>0.4072916666666666</v>
       </c>
       <c r="E82" t="n">
-        <v>0.4327913226694187</v>
+        <v>0</v>
       </c>
       <c r="F82" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="G82" t="n">
-        <v>0.5927083333333333</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="83">
@@ -2602,19 +2354,16 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>0.584375</v>
+        <v>0.4245789473684209</v>
       </c>
       <c r="D83" t="n">
-        <v>1</v>
+        <v>0.4156249999999999</v>
       </c>
       <c r="E83" t="n">
-        <v>0.4245789473684209</v>
+        <v>0</v>
       </c>
       <c r="F83" t="n">
-        <v>0.6354166666666666</v>
-      </c>
-      <c r="G83" t="n">
-        <v>0.584375</v>
+        <v>0.3645833333333334</v>
       </c>
     </row>
     <row r="84">
@@ -2629,19 +2378,16 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>0.5750000000000001</v>
+        <v>0.4791434468524252</v>
       </c>
       <c r="D84" t="n">
-        <v>1</v>
+        <v>0.4249999999999999</v>
       </c>
       <c r="E84" t="n">
-        <v>0.4791434468524252</v>
+        <v>0</v>
       </c>
       <c r="F84" t="n">
-        <v>0.6698113207547169</v>
-      </c>
-      <c r="G84" t="n">
-        <v>0.5750000000000001</v>
+        <v>0.3301886792452831</v>
       </c>
     </row>
     <row r="85">
@@ -2656,19 +2402,16 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>0.5885416666666666</v>
+        <v>0.4491990269792127</v>
       </c>
       <c r="D85" t="n">
-        <v>1</v>
+        <v>0.4114583333333333</v>
       </c>
       <c r="E85" t="n">
-        <v>0.4491990269792127</v>
+        <v>0</v>
       </c>
       <c r="F85" t="n">
-        <v>0.7350427350427351</v>
-      </c>
-      <c r="G85" t="n">
-        <v>0.5885416666666666</v>
+        <v>0.2649572649572649</v>
       </c>
     </row>
     <row r="86">
@@ -2683,19 +2426,16 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>0.5645833333333333</v>
+        <v>0.4321666666666666</v>
       </c>
       <c r="D86" t="n">
-        <v>1</v>
+        <v>0.4354166666666667</v>
       </c>
       <c r="E86" t="n">
-        <v>0.4321666666666666</v>
+        <v>0</v>
       </c>
       <c r="F86" t="n">
-        <v>0.6354166666666666</v>
-      </c>
-      <c r="G86" t="n">
-        <v>0.5645833333333333</v>
+        <v>0.3645833333333334</v>
       </c>
     </row>
     <row r="87">
@@ -2710,19 +2450,16 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>0.5822916666666667</v>
+        <v>0.450483660130719</v>
       </c>
       <c r="D87" t="n">
-        <v>1</v>
+        <v>0.4177083333333334</v>
       </c>
       <c r="E87" t="n">
-        <v>0.450483660130719</v>
+        <v>0</v>
       </c>
       <c r="F87" t="n">
-        <v>0.6850393700787402</v>
-      </c>
-      <c r="G87" t="n">
-        <v>0.5822916666666667</v>
+        <v>0.3149606299212598</v>
       </c>
     </row>
     <row r="88">
@@ -2737,19 +2474,16 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>0.5781249999999999</v>
+        <v>0.429233660130719</v>
       </c>
       <c r="D88" t="n">
-        <v>1</v>
+        <v>0.421875</v>
       </c>
       <c r="E88" t="n">
-        <v>0.429233660130719</v>
+        <v>0</v>
       </c>
       <c r="F88" t="n">
-        <v>0.6854838709677419</v>
-      </c>
-      <c r="G88" t="n">
-        <v>0.578125</v>
+        <v>0.3145161290322581</v>
       </c>
     </row>
     <row r="89">
@@ -2764,19 +2498,16 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>0.5927083333333333</v>
+        <v>0.5069705882352943</v>
       </c>
       <c r="D89" t="n">
-        <v>1</v>
+        <v>0.4072916666666667</v>
       </c>
       <c r="E89" t="n">
-        <v>0.5069705882352943</v>
+        <v>0</v>
       </c>
       <c r="F89" t="n">
-        <v>0.6458333333333334</v>
-      </c>
-      <c r="G89" t="n">
-        <v>0.5927083333333333</v>
+        <v>0.3541666666666666</v>
       </c>
     </row>
     <row r="90">
@@ -2791,19 +2522,16 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>0.5843749999999999</v>
+        <v>0.4466482628138976</v>
       </c>
       <c r="D90" t="n">
-        <v>1</v>
+        <v>0.4156250000000001</v>
       </c>
       <c r="E90" t="n">
-        <v>0.4466482628138976</v>
+        <v>0</v>
       </c>
       <c r="F90" t="n">
-        <v>0.7086614173228346</v>
-      </c>
-      <c r="G90" t="n">
-        <v>0.5843749999999999</v>
+        <v>0.2913385826771654</v>
       </c>
     </row>
     <row r="91">
@@ -2818,19 +2546,16 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>0.5864583333333333</v>
+        <v>0.4145497076023393</v>
       </c>
       <c r="D91" t="n">
-        <v>1</v>
+        <v>0.4135416666666666</v>
       </c>
       <c r="E91" t="n">
-        <v>0.4145497076023393</v>
+        <v>0</v>
       </c>
       <c r="F91" t="n">
-        <v>0.6825396825396826</v>
-      </c>
-      <c r="G91" t="n">
-        <v>0.5864583333333333</v>
+        <v>0.3174603174603174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>